<commit_message>
Namen der Tabellen und Spalten angepasst (Sprache geändert, deutsch -> englisch)
</commit_message>
<xml_diff>
--- a/Datenbank/Datenbank_v1.xlsx
+++ b/Datenbank/Datenbank_v1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{527AE4C7-C243-4703-8940-F6EB9E4FF97A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C165FA75-B7A5-46F2-8D1A-801057EA9045}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,20 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="43">
   <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>ID_Admin</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Passwort</t>
-  </si>
-  <si>
     <t>Bezeichnung</t>
   </si>
   <si>
@@ -71,87 +62,18 @@
     <t>Verschlüsselung</t>
   </si>
   <si>
-    <t>Azubi</t>
-  </si>
-  <si>
-    <t>ID_Azubi</t>
-  </si>
-  <si>
-    <t>Login-Code</t>
-  </si>
-  <si>
-    <t>Ansprechpartner</t>
-  </si>
-  <si>
-    <t>ID_Ansprechpartner</t>
-  </si>
-  <si>
     <t>Anmerkung</t>
   </si>
   <si>
-    <t>Benutzer</t>
-  </si>
-  <si>
     <t>Firmen E-Mail</t>
   </si>
   <si>
-    <t>Nachname</t>
-  </si>
-  <si>
-    <t>Vorname</t>
-  </si>
-  <si>
-    <t>ID_Standort</t>
-  </si>
-  <si>
     <t>Foreign Key</t>
   </si>
   <si>
-    <t>Beschreibung</t>
-  </si>
-  <si>
     <t>---</t>
   </si>
   <si>
-    <t>Bild</t>
-  </si>
-  <si>
-    <t>ID_Lehrtyp</t>
-  </si>
-  <si>
-    <t>Erstellungsdatum</t>
-  </si>
-  <si>
-    <t>Timestamp</t>
-  </si>
-  <si>
-    <t>8/10/15:19</t>
-  </si>
-  <si>
-    <t>Alter</t>
-  </si>
-  <si>
-    <t>Stadt</t>
-  </si>
-  <si>
-    <t>Standort</t>
-  </si>
-  <si>
-    <t>Lehrtyp</t>
-  </si>
-  <si>
-    <t>Beruf</t>
-  </si>
-  <si>
-    <t>ID_Beruf</t>
-  </si>
-  <si>
-    <t>E-Mail</t>
-  </si>
-  <si>
-    <t>Freitext-Kontaktmöglichkeit</t>
-  </si>
-  <si>
     <t>JA (Ansprechpartner)</t>
   </si>
   <si>
@@ -162,6 +84,75 @@
   </si>
   <si>
     <t>JA (Beruf)</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Trainee</t>
+  </si>
+  <si>
+    <t>Godfather</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>Hiring_Date</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
+    <t>Pick_Text</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Teaching_Type</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>User_Name</t>
+  </si>
+  <si>
+    <t>Login_Code</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Id_Location</t>
+  </si>
+  <si>
+    <t>Id_Teaching_Type</t>
+  </si>
+  <si>
+    <t>Id_Job</t>
+  </si>
+  <si>
+    <t>Id_Godfather</t>
+  </si>
+  <si>
+    <t>Id_Trainee</t>
+  </si>
+  <si>
+    <t>Id_Admin</t>
   </si>
 </sst>
 </file>
@@ -505,7 +496,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,31 +513,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -557,260 +548,260 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>500</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <v>500</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C19">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <v>5000</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -818,158 +809,152 @@
         <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C23">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C26">
         <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>500</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C30">
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C31">
         <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C34">
         <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G34" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C35">
         <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -977,33 +962,33 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C38">
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G38" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C39">
         <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Datentyp und Größe der Spalte Picture angepasst
</commit_message>
<xml_diff>
--- a/Datenbank/Datenbank_v1.xlsx
+++ b/Datenbank/Datenbank_v1.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C165FA75-B7A5-46F2-8D1A-801057EA9045}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DC0FCFA6-6FB0-4A29-8EF4-E57E96644270}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="41">
   <si>
     <t>Admin</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Foreign Key</t>
   </si>
   <si>
-    <t>---</t>
-  </si>
-  <si>
     <t>JA (Ansprechpartner)</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
   </si>
   <si>
     <t>Job</t>
-  </si>
-  <si>
-    <t>User_Name</t>
   </si>
   <si>
     <t>Login_Code</t>
@@ -493,10 +487,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,7 +543,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -582,7 +577,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -600,12 +595,12 @@
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -625,7 +620,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -639,7 +634,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -651,18 +646,18 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -682,7 +677,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -699,7 +694,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -716,7 +711,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -730,7 +725,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -744,7 +739,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -756,12 +751,12 @@
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>10</v>
@@ -775,13 +770,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="C21" s="3">
+        <v>20</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -789,7 +784,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -801,12 +796,12 @@
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -818,15 +813,15 @@
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
         <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>26</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
@@ -834,10 +829,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -845,7 +840,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
@@ -859,7 +854,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -874,12 +869,12 @@
     <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
@@ -899,7 +894,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -914,12 +909,12 @@
     <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
@@ -939,7 +934,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
@@ -954,12 +949,12 @@
     <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
@@ -979,7 +974,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
View Doku hinzugefügt, Dokument zum erstellen der Views hinzugefügt, Datenbank_v1 aktualisiert
</commit_message>
<xml_diff>
--- a/Datenbank/Datenbank_v1.xlsx
+++ b/Datenbank/Datenbank_v1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DC0FCFA6-6FB0-4A29-8EF4-E57E96644270}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EB892F44-FE21-42B8-9C3E-2B3E8BE091C6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,8 +11,8 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="A2000381">Tabelle1!$A$1000379</definedName>
-    <definedName name="A9999999">Tabelle1!$A$99997</definedName>
+    <definedName name="A2000381">Tabelle1!$A$1000378</definedName>
+    <definedName name="A9999999">Tabelle1!$A$99996</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="41">
   <si>
     <t>Admin</t>
   </si>
@@ -488,10 +488,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -840,149 +840,135 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
       <c r="C26">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27">
-        <v>500</v>
-      </c>
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C30">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
       </c>
-      <c r="E30" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31">
-        <v>50</v>
-      </c>
-      <c r="D31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="31" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C34">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
       </c>
-      <c r="E34" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35">
-        <v>50</v>
-      </c>
-      <c r="D35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C38">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39">
-        <v>50</v>
-      </c>
-      <c r="D39" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>